<commit_message>
updated valid and invalid code updated
</commit_message>
<xml_diff>
--- a/src/test/resources/data/input.xlsx
+++ b/src/test/resources/data/input.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\B24\Day32 Dec22\B24\src\test\resources\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CB9E03-5BD8-4686-BE29-B890618F304B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="615" windowWidth="15255" windowHeight="9030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5070" yWindow="615" windowWidth="15255" windowHeight="9030" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="InvalidLogin" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,16 +20,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>FailMsg</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>Home Page is not displayed</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,7 +141,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -160,7 +176,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -337,25 +353,82 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>